<commit_message>
hw results 13 14
</commit_message>
<xml_diff>
--- a/Results_P3.xlsx
+++ b/Results_P3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\courses\python_Boot_camp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4FAD06-ACBE-4751-B88A-51E36AD1D426}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953EFE13-52C7-4A47-84FF-EB835938BD3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1200" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Петрович Оксана</t>
   </si>
@@ -108,20 +108,41 @@
     <t>4(too late)</t>
   </si>
   <si>
-    <t>4 (перегрузка отлично, однако такой вариант, например for i in ranger(1,10,-2):
+    <t>5(чтобы csv строки не имели пропуска есть параметр newline)</t>
+  </si>
+  <si>
+    <t>5 (well done)</t>
+  </si>
+  <si>
+    <t>4(late)</t>
+  </si>
+  <si>
+    <t>5 (Некоторые использовали openweather api чтобы их не блокировали)</t>
+  </si>
+  <si>
+    <t>4 (перегрузка отлично, однако такой вариант, например for i in range(1,10,-2): не работает
     print(i) даст неправильный результат)</t>
   </si>
   <si>
-    <t>5(чтобы csv строки не имели пропуска есть параметр newline)</t>
-  </si>
-  <si>
-    <t>5 (well done)</t>
-  </si>
-  <si>
-    <t>4(late)</t>
-  </si>
-  <si>
-    <t>5 (Некоторые использовали openweather api чтобы их не блокировали)</t>
+    <t>№14</t>
+  </si>
+  <si>
+    <t>№15</t>
+  </si>
+  <si>
+    <t>№16</t>
+  </si>
+  <si>
+    <t>5(Хотелось бы все таки небольшой отчет)</t>
+  </si>
+  <si>
+    <t>5 (Можно попробовать оптимизировать работу на процессах. Например, каждый процесс может обрабатывать несколько каких-то вещей сразу. Массив, например)</t>
+  </si>
+  <si>
+    <t>5 (openweather можно использовать)</t>
+  </si>
+  <si>
+    <t>5 (Для ускорения можно совмещать многопроцесный вариант и асинхронный например)</t>
   </si>
 </sst>
 </file>
@@ -456,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -467,7 +488,7 @@
     <col min="1" max="1" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -507,8 +528,17 @@
       <c r="N1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -548,8 +578,14 @@
       <c r="M2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -589,8 +625,14 @@
       <c r="M3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -619,19 +661,25 @@
         <v>26</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L4">
         <v>5</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -671,8 +719,14 @@
       <c r="M5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -712,9 +766,15 @@
       <c r="M6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7">
@@ -744,8 +804,8 @@
       <c r="J7">
         <v>5</v>
       </c>
-      <c r="K7">
-        <v>0</v>
+      <c r="K7" t="s">
+        <v>29</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -753,8 +813,14 @@
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -774,10 +840,10 @@
         <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -794,9 +860,15 @@
       <c r="M8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -832,11 +904,17 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,8 +954,14 @@
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -912,16 +996,25 @@
         <v>5</v>
       </c>
       <c r="L11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" t="s">
         <v>28</v>
       </c>
-      <c r="M11" t="s">
-        <v>29</v>
-      </c>
       <c r="N11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+      <c r="P11">
+        <v>5</v>
+      </c>
+      <c r="Q11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -961,8 +1054,14 @@
       <c r="M12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N12">
+        <v>5</v>
+      </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1001,6 +1100,18 @@
       </c>
       <c r="M13">
         <v>5</v>
+      </c>
+      <c r="N13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
+      <c r="P13">
+        <v>5</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>